<commit_message>
Changed the HTML generation considerably, added bagging option when generating HTML, added zipping option but only when generating HTML. Broke a couple of tests. The bag metadata generation needs to be moved to bag.js and that will help
</commit_message>
<xml_diff>
--- a/test_data/Glop_Pot/datasheets/CATALOG_datasheets.xlsx
+++ b/test_data/Glop_Pot/datasheets/CATALOG_datasheets.xlsx
@@ -392,7 +392,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Title</v>
+        <v>Name</v>
       </c>
       <c r="B2" t="str">
         <v xml:space="preserve">CP7 Glop Pot, Cooleman Plains, Glop Pot data sheets </v>
@@ -400,7 +400,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Organisation</v>
+        <v>Organization</v>
       </c>
       <c r="B3" t="str">
         <v>Sydney University Speleological Society</v>

</xml_diff>

<commit_message>
More improvements to index.html - still one test failing, but the output is correct when called from commandline
</commit_message>
<xml_diff>
--- a/test_data/Glop_Pot/datasheets/CATALOG_datasheets.xlsx
+++ b/test_data/Glop_Pot/datasheets/CATALOG_datasheets.xlsx
@@ -414,7 +414,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Files"/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -432,9 +432,6 @@
       <c r="D1" t="str">
         <v>RELATION:License</v>
       </c>
-      <c r="E1" t="str">
-        <v>*MISSING-FILE*</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -464,30 +461,6 @@
         <v>CC-BY</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>metadata.ods</v>
-      </c>
-      <c r="E4" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>CATALOG.xlsx</v>
-      </c>
-      <c r="E5" t="str">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>CATALOG_datasheets.xlsx</v>
-      </c>
-      <c r="E6" t="str">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>